<commit_message>
Tesing and fixing bugs
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BD2500-7ED9-497C-A4E7-8F92EAFE727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA62CE77-1151-40F8-B326-D1464E35CC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1236" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>["https://finance.yahoo.com/markets/stocks/most-active/","https://finance.yahoo.com/markets/stocks/trending/","https://finance.yahoo.com/markets/stocks/gainers/","https://finance.yahoo.com/markets/stocks/losers/"]</t>
+  </si>
+  <si>
+    <t>ExtractLimitFromURL</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -505,6 +508,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>

</xml_diff>

<commit_message>
Implemented Data Storage in Excel workbook
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEAF0C8-FA86-4EDB-924E-2CF46C844283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E6747A-DCBA-4D41-AE6C-5E9F0EEC65A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1236" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Fix bugs and add logs
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E6747A-DCBA-4D41-AE6C-5E9F0EEC65A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1313DA-3414-4092-B76E-82C64D1A1720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1236" yWindow="624" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -69,12 +69,6 @@
     <t>Data\Output</t>
   </si>
   <si>
-    <t>TrendingUrlTemplate</t>
-  </si>
-  <si>
-    <t>https://query1.finance.yahoo.com/v1/finance/trending/US?lang=en-US&amp;region=US&amp;count={count}&amp;corsDomain=finance.yahoo.com</t>
-  </si>
-  <si>
     <t>ExtractDataFromUrl</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>["https://finance.yahoo.com/markets/stocks/trending/","https://finance.yahoo.com/markets/stocks/gainers/","https://finance.yahoo.com/markets/stocks/losers/"]</t>
+  </si>
+  <si>
+    <t>YahooFinanceUrl</t>
+  </si>
+  <si>
+    <t>https://finance.yahoo.com/</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -494,23 +494,23 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -519,8 +519,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{76229C46-E61F-46B7-955F-557827B01F03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented HTML formatted email report and Send Email
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1313DA-3414-4092-B76E-82C64D1A1720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E8884-1CA0-417D-9487-F7A392C80763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="15600" windowWidth="19068" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -33,18 +33,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>OutputFilePath</t>
-  </si>
-  <si>
-    <t>Data\Output\Results.xlsx</t>
-  </si>
-  <si>
-    <t>OutputSheetName</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
     <t>ScreenshotsFolder</t>
   </si>
   <si>
@@ -82,6 +70,12 @@
   </si>
   <si>
     <t>https://finance.yahoo.com/</t>
+  </si>
+  <si>
+    <t>matan10cohen@gmail.com</t>
+  </si>
+  <si>
+    <t>MailRecipient</t>
   </si>
 </sst>
 </file>
@@ -416,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -438,10 +432,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -464,64 +458,57 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
+      <c r="B9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>14</v>
+      <c r="A10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{76229C46-E61F-46B7-955F-557827B01F03}"/>
+    <hyperlink ref="B8" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{76229C46-E61F-46B7-955F-557827B01F03}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{09B06EAA-0331-4BC0-BF43-C4B34D588381}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Logging - The log file does not updated
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\OneDrive\Documents\UiPath\AutomatingFinancialData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1E8884-1CA0-417D-9487-F7A392C80763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00433BF0-C7D2-4613-BB3F-69D60CBC14EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="15600" windowWidth="19068" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -33,22 +33,7 @@
     <t>Value</t>
   </si>
   <si>
-    <t>ScreenshotsFolder</t>
-  </si>
-  <si>
-    <t>Screenshots</t>
-  </si>
-  <si>
-    <t>LogFilePath</t>
-  </si>
-  <si>
-    <t>Logs\run.log</t>
-  </si>
-  <si>
     <t>TopMoversThresholdPercent</t>
-  </si>
-  <si>
-    <t>MaxTickersToProcess</t>
   </si>
   <si>
     <t>OutputFolder</t>
@@ -410,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -432,81 +417,57 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>13</v>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{76229C46-E61F-46B7-955F-557827B01F03}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{09B06EAA-0331-4BC0-BF43-C4B34D588381}"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://ca.finance.yahoo.com/markets/stocks/most-active/" xr:uid="{B54C4B8B-5F17-4D15-9A3F-F19708E662C7}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{76229C46-E61F-46B7-955F-557827B01F03}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{09B06EAA-0331-4BC0-BF43-C4B34D588381}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>